<commit_message>
Add sentry and improve http log
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chunlee\Desktop\Projects\Flutter\flutter_boiler_plate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916CB57C-FFCB-464B-BC0B-4CB20D78AF1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0677901-CA23-4CD9-909B-728A5086948A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E323C134-2CB6-4AA9-8D83-F91A0034127A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E323C134-2CB6-4AA9-8D83-F91A0034127A}"/>
   </bookViews>
   <sheets>
     <sheet name="Translation" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="126">
   <si>
     <t>key</t>
   </si>
@@ -352,13 +352,70 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>រក្សាទុក</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>លុប</t>
+  </si>
+  <si>
+    <t>អ្នកប្រើប្រាស់</t>
+  </si>
+  <si>
+    <t>ម៉ោង</t>
+  </si>
+  <si>
+    <t>ខែ</t>
+  </si>
+  <si>
+    <t>ទៅ</t>
+  </si>
+  <si>
+    <t>ពី</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,13 +425,21 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Khmer OS Bokor"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Khmer OS System"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -414,17 +479,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,418 +805,499 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F4463F-CE2E-4F97-AE4C-A51824482920}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="43" defaultRowHeight="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="42.5703125" defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="43" style="1"/>
+    <col min="1" max="1" width="42.5703125" style="3"/>
+    <col min="2" max="2" width="87.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="98.5703125" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="42.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C36">
     <sortCondition ref="A1"/>
   </sortState>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>